<commit_message>
Process migration to LT-00179
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20363"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arjun.shenoy\Documents\UiPath\Screener_EXCEL\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arjun.shenoy\Documents\UiPath\StockMarketAnalysis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C3039A-D7AB-4608-9047-A63FF6E8B269}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1BC639-6209-4860-A37F-88931A540E7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -588,7 +588,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>